<commit_message>
update 5 april 2020
</commit_message>
<xml_diff>
--- a/sicilia/covid19-regione-sicilia.xlsx
+++ b/sicilia/covid19-regione-sicilia.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/digangi/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/digangi/COVID19-Monitor/sicilia/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="9620" yWindow="2920" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -86,7 +86,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -136,12 +136,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Migliaia" xfId="1" builtinId="3"/>
@@ -423,7 +426,7 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C2" sqref="C2:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -479,6 +482,24 @@
       <c r="B2" s="2">
         <v>434870</v>
       </c>
+      <c r="C2" s="5">
+        <v>104</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5">
+        <v>2</v>
+      </c>
+      <c r="F2" s="5">
+        <v>1</v>
+      </c>
+      <c r="G2" s="5">
+        <v>107</v>
+      </c>
+      <c r="H2" s="5">
+        <v>104</v>
+      </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="4"/>
@@ -493,6 +514,24 @@
       <c r="B3" s="2">
         <v>262458</v>
       </c>
+      <c r="C3" s="5">
+        <v>91</v>
+      </c>
+      <c r="D3" s="5">
+        <v>23</v>
+      </c>
+      <c r="E3" s="5">
+        <v>4</v>
+      </c>
+      <c r="F3" s="5">
+        <v>7</v>
+      </c>
+      <c r="G3" s="5">
+        <v>102</v>
+      </c>
+      <c r="H3" s="5">
+        <v>68</v>
+      </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -507,6 +546,24 @@
       <c r="B4" s="2">
         <v>1107702</v>
       </c>
+      <c r="C4" s="5">
+        <v>525</v>
+      </c>
+      <c r="D4" s="5">
+        <v>153</v>
+      </c>
+      <c r="E4" s="5">
+        <v>23</v>
+      </c>
+      <c r="F4" s="5">
+        <v>46</v>
+      </c>
+      <c r="G4" s="5">
+        <v>594</v>
+      </c>
+      <c r="H4" s="5">
+        <v>372</v>
+      </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -521,6 +578,24 @@
       <c r="B5" s="2">
         <v>164788</v>
       </c>
+      <c r="C5" s="5">
+        <v>270</v>
+      </c>
+      <c r="D5" s="5">
+        <v>170</v>
+      </c>
+      <c r="E5" s="5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5">
+        <v>13</v>
+      </c>
+      <c r="G5" s="5">
+        <v>284</v>
+      </c>
+      <c r="H5" s="5">
+        <v>100</v>
+      </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -535,6 +610,24 @@
       <c r="B6" s="2">
         <v>626876</v>
       </c>
+      <c r="C6" s="5">
+        <v>314</v>
+      </c>
+      <c r="D6" s="5">
+        <v>138</v>
+      </c>
+      <c r="E6" s="5">
+        <v>15</v>
+      </c>
+      <c r="F6" s="5">
+        <v>24</v>
+      </c>
+      <c r="G6" s="5">
+        <v>353</v>
+      </c>
+      <c r="H6" s="5">
+        <v>176</v>
+      </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -549,7 +642,24 @@
       <c r="B7" s="2">
         <v>1252588</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="5">
+        <v>258</v>
+      </c>
+      <c r="D7" s="5">
+        <v>73</v>
+      </c>
+      <c r="E7" s="5">
+        <v>29</v>
+      </c>
+      <c r="F7" s="5">
+        <v>12</v>
+      </c>
+      <c r="G7" s="5">
+        <v>299</v>
+      </c>
+      <c r="H7" s="5">
+        <v>185</v>
+      </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -564,6 +674,24 @@
       <c r="B8" s="2">
         <v>320893</v>
       </c>
+      <c r="C8" s="5">
+        <v>41</v>
+      </c>
+      <c r="D8" s="5">
+        <v>7</v>
+      </c>
+      <c r="E8" s="5">
+        <v>4</v>
+      </c>
+      <c r="F8" s="5">
+        <v>3</v>
+      </c>
+      <c r="G8" s="5">
+        <v>48</v>
+      </c>
+      <c r="H8" s="5">
+        <v>34</v>
+      </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -578,6 +706,24 @@
       <c r="B9" s="2">
         <v>399224</v>
       </c>
+      <c r="C9" s="5">
+        <v>77</v>
+      </c>
+      <c r="D9" s="5">
+        <v>44</v>
+      </c>
+      <c r="E9" s="5">
+        <v>25</v>
+      </c>
+      <c r="F9" s="5">
+        <v>7</v>
+      </c>
+      <c r="G9" s="5">
+        <v>109</v>
+      </c>
+      <c r="H9" s="5">
+        <v>33</v>
+      </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -592,6 +738,24 @@
       <c r="B10" s="2">
         <v>430492</v>
       </c>
+      <c r="C10" s="5">
+        <v>94</v>
+      </c>
+      <c r="D10" s="5">
+        <v>24</v>
+      </c>
+      <c r="E10" s="5">
+        <v>1</v>
+      </c>
+      <c r="F10" s="5">
+        <v>3</v>
+      </c>
+      <c r="G10" s="5">
+        <v>98</v>
+      </c>
+      <c r="H10" s="5">
+        <v>70</v>
+      </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>

</xml_diff>